<commit_message>
Gehele Backlog van sprint 0 t/m 3
</commit_message>
<xml_diff>
--- a/Documentatie/Product_Backlog_Completed.xlsx
+++ b/Documentatie/Product_Backlog_Completed.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9090"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9090" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="PRODUCT BACKLOG + PLANNING" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="93">
   <si>
     <t>SPRINT 1 BACKLOG</t>
   </si>
@@ -222,14 +222,146 @@
     <t>SPRINT 0 BACKLOG</t>
   </si>
   <si>
-    <t>[]</t>
+    <t xml:space="preserve">Als P.O wil ik een usecase diagram zien zodat ik een overzicht heb welke eisen er aan het eindproduct zitten. </t>
+  </si>
+  <si>
+    <t>Als gebruiker van de applicatie wil ik een aantrekkelijk design zodat ik het prettig vind om de app te bekijken.</t>
+  </si>
+  <si>
+    <t>[20]</t>
+  </si>
+  <si>
+    <t>1. Achter haal alle gebruikers en 3e partijen
+2. Achterhaal de eisen van de gebruiker
+3. Maak de connecties tussen gebruiker en eis</t>
+  </si>
+  <si>
+    <t>1. Er zijn gebruikers en 3e partijen gedefineerd
+2. De eisen van de gebruiker zijn gedefineerd 
+3. Er is een duidelijke connectie tussen gebruikers en eisen</t>
+  </si>
+  <si>
+    <t>1. Bedenk welke kleuren en vormgeving je wilt toepassen. 
+2. Welke schermen heeft de applicatie. 
+3. Voeg animatie toe aan de applicatie. 
+4. Programmeer het design van de verschillende schermen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. De kleuren zijn op elkaar afgestemd en aantrekkelijk. 
+2. De vormgeving is rustgevend en overzichtelijk. 
+3. Het design is aantrekkelijk gemaakt met animaties. 
+4. De verschillende schermen zijn op elkaar afgestemd. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Als gebruiker wil ik des betreffende data op de app kunnen zien zodat ik de app kan gebruiken waarvoor die gemaakt is. </t>
+  </si>
+  <si>
+    <t>1. Verzamel data over de parkeergelegenheden. 
+2. Verzamel data over de oplaadpalen. 
+3. Weergeef deze informatie in Java.</t>
+  </si>
+  <si>
+    <t>1. Beschik over de volledige data van de parkeergelegenheden.
+2. Beschik over de volledige data van de oplaadpalen. 
+3. Alle data die is verzameld is verwerkt in Java</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Als developer wil ik een ERD(Entity Relationship Diagram) hebben zodat ik een beeld heb hoe de database eruit komt te zien. </t>
+  </si>
+  <si>
+    <t>[7]</t>
+  </si>
+  <si>
+    <t>Als gebruiker wil ik dat de data die ik op mijn app kan bekijken aan elkaar gekoppeld is zodat ik de data apart maar ook gezamenlijk kan checken.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Als gebruiker wil ik de data visueel op mijn applicatie zien zodat ik op de kaart van Rotterdam makkelijk kan zien waar ik kan parkeren en mijn auto kan opladen. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Als developer wil ik de data in de database hebben zodat ik de data kan opslaan, combineren en gebruiken. </t>
+  </si>
+  <si>
+    <t>[13]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Bepaal welke entities er zijn. 
+2. Bepaal de attributes van deze entities.
+3. Maak de relationship tussen de verschillende entities. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Zorg dat de entities duidelijk zijn, met een goede benaming en met de juiste attributes. 
+2. Zorg dat de relationship tussen de entities duidelijk zijn en goed geformuleerd. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Filter de verzamelde data op de stad Rotterdam.
+2. Combineer de 2 verschillende soorten data's met elkaar.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. De data gaat alleen over de stad Rotterdam. 
+2. De 2 verschillende soorten data's hebben een connectie met elkaar. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Zorg dat de verzamelde data op de app af te lezen is. 
+2. Zorg dat de kaart met de data klopt. 
+3. Zorg dat de animatie met de data klopt. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. De data is zichtbaar op de applicatie. 
+2. De verschillende schermen tonen de juiste data. 
+3. Op de kaart wordt de juiste data getoond. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Maak een database aan voor de parkeergelegenheden. 
+2. Maak een database aan voor de oplaadpalen. 
+3. Filter deze op stad. 
+4. Maak een connectie met de database. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. De database bestaat uit 2 soorten data: de parkeergelegenheden en de oplaadpalen.
+2. De database valt te filteren op steden. 
+3. Er is een goede connectie tussen applicatie en database. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Als developer wil ik een classe diagram zien zodat ik een overzicht heb van de structeer(classes, methods etc.) van het programma. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">als P.O wil ik een activity diagram zien zodat ik een duidelijk overzicht heb hoe het programma tot zijn einddoel komt. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Als gebruiker wil ik dat Google maps API in de applicatie is verwerkt zodat ik de kaart op de applicatie kan tonen en zo de weg kan vinden naar de parkeergarages of oplaadpunten. </t>
+  </si>
+  <si>
+    <t>1. Maak een overzicht van alle classes en welke informatie deze classes bevatten. 
+2. Laat de connectie zien tussen de verschillende classes.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Een goed overzichtelijke diagram waar je de classes in kan vinden met zijn informatie en methodes. 
+2. De classes moeten een goede connectie met elkaar hebben. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Ga na wat alle stappen zijn die het programma maakt. 
+2. Zorg dat deze stappen overzichtelijk met elkaar verbonden zijn. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Een goed overzichtelijke diagram waar je stap voor stap kan zien hoe het programma verloopt.
+2. Er moet time managment in zitten. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Voeg de kaart toe aan applicatie.
+2. Zorg dat de data op de kaart kan worden getoond. 
+3. Maak de kaart toegankelijk voor de gebruiker. </t>
+  </si>
+  <si>
+    <t>1. De kaart is verwerkt in de applicatie. 
+2. De gebruiker kan gebruik maken van deze kaart. 
+3. De data wordt getoond op de kaart.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -330,6 +462,20 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -482,7 +628,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="4" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -614,23 +760,8 @@
     <xf numFmtId="49" fontId="2" fillId="5" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="5" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="16" fillId="5" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="5" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="16" fillId="5" borderId="8" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -640,6 +771,12 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="5" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="8" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -652,11 +789,36 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="8" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="8" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -975,11 +1137,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE1006"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C17" sqref="C17"/>
+      <selection pane="bottomRight" activeCell="B15" sqref="B15:B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -995,10 +1157,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="40.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="55"/>
+      <c r="B1" s="52"/>
       <c r="C1" s="1"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
@@ -34372,7 +34534,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -34386,10 +34548,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="51" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="56"/>
+      <c r="B1" s="53"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -34479,7 +34641,7 @@
       <c r="A6" s="36">
         <v>3</v>
       </c>
-      <c r="B6" s="52" t="s">
+      <c r="B6" s="47" t="s">
         <v>41</v>
       </c>
       <c r="C6" s="37" t="s">
@@ -34491,7 +34653,7 @@
       <c r="E6" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="F6" s="53" t="s">
+      <c r="F6" s="48" t="s">
         <v>50</v>
       </c>
     </row>
@@ -34511,7 +34673,7 @@
       <c r="E7" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="F7" s="53" t="s">
+      <c r="F7" s="48" t="s">
         <v>52</v>
       </c>
     </row>
@@ -34598,7 +34760,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -34606,15 +34768,15 @@
     <col min="1" max="1" width="8.85546875" style="20"/>
     <col min="2" max="2" width="35.7109375" customWidth="1"/>
     <col min="3" max="4" width="8.85546875" style="19"/>
-    <col min="5" max="5" width="40.7109375" customWidth="1"/>
-    <col min="6" max="6" width="35.28515625" customWidth="1"/>
+    <col min="5" max="5" width="50.7109375" customWidth="1"/>
+    <col min="6" max="6" width="52.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="26.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="58"/>
+      <c r="B1" s="55"/>
       <c r="C1" s="22"/>
       <c r="D1" s="22"/>
       <c r="E1" s="23"/>
@@ -34640,69 +34802,90 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="59">
+    <row r="3" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="49">
         <v>5</v>
       </c>
-      <c r="B3" s="46"/>
+      <c r="B3" s="41" t="s">
+        <v>60</v>
+      </c>
       <c r="C3" s="42" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="43" t="s">
-        <v>60</v>
+        <v>12</v>
       </c>
-      <c r="E3" s="44"/>
-      <c r="F3" s="45"/>
-    </row>
-    <row r="4" spans="1:6" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="59">
+      <c r="E3" s="57" t="s">
+        <v>63</v>
+      </c>
+      <c r="F3" s="57" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="49">
         <v>6</v>
       </c>
-      <c r="B4" s="47"/>
+      <c r="B4" s="56" t="s">
+        <v>61</v>
+      </c>
       <c r="C4" s="41" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="41" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
+      <c r="E4" s="44" t="s">
+        <v>65</v>
+      </c>
+      <c r="F4" s="44" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="5" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="59">
+      <c r="A5" s="49">
         <v>7</v>
       </c>
-      <c r="B5" s="46"/>
+      <c r="B5" s="41" t="s">
+        <v>67</v>
+      </c>
       <c r="C5" s="41" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="41" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
+      <c r="E5" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="F5" s="44" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6"/>
       <c r="C6"/>
       <c r="D6"/>
     </row>
-    <row r="7" spans="1:6" ht="61.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7"/>
+      <c r="B7" s="13"/>
       <c r="C7"/>
       <c r="D7"/>
     </row>
-    <row r="8" spans="1:6" ht="160.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8"/>
+      <c r="B8" s="10"/>
       <c r="C8"/>
       <c r="D8"/>
     </row>
-    <row r="9" spans="1:6" ht="73.150000000000006" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9"/>
+      <c r="B9" s="13"/>
       <c r="C9"/>
       <c r="D9"/>
     </row>
-    <row r="10" spans="1:6" ht="135.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10"/>
       <c r="C10"/>
       <c r="D10"/>
@@ -34744,22 +34927,184 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="35.7109375" customWidth="1"/>
-    <col min="5" max="5" width="35.5703125" customWidth="1"/>
-    <col min="6" max="6" width="35.28515625" customWidth="1"/>
+    <col min="5" max="5" width="50.42578125" customWidth="1"/>
+    <col min="6" max="6" width="47.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="26.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="55"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+    </row>
+    <row r="2" spans="1:6" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="61" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="62" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="62" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="63">
+        <v>8</v>
+      </c>
+      <c r="B3" s="64" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" s="64" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="64" t="s">
+        <v>71</v>
+      </c>
+      <c r="E3" s="65" t="s">
+        <v>76</v>
+      </c>
+      <c r="F3" s="65" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="63">
+        <v>9</v>
+      </c>
+      <c r="B4" s="64" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" s="64" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="64" t="s">
+        <v>75</v>
+      </c>
+      <c r="E4" s="65" t="s">
+        <v>78</v>
+      </c>
+      <c r="F4" s="65" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="63">
+        <v>10</v>
+      </c>
+      <c r="B5" s="64" t="s">
+        <v>73</v>
+      </c>
+      <c r="C5" s="64" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="64" t="s">
+        <v>75</v>
+      </c>
+      <c r="E5" s="65" t="s">
+        <v>80</v>
+      </c>
+      <c r="F5" s="65" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="68.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="63">
+        <v>11</v>
+      </c>
+      <c r="B6" s="64" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" s="64" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="64" t="s">
+        <v>62</v>
+      </c>
+      <c r="E6" s="65" t="s">
+        <v>82</v>
+      </c>
+      <c r="F6" s="66" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="13"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B9" s="13"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B10" s="13"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B11" s="13"/>
+    </row>
+    <row r="12" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="21"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+    </row>
+    <row r="13" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="21"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="35.7109375" customWidth="1"/>
+    <col min="5" max="5" width="45.7109375" customWidth="1"/>
+    <col min="6" max="6" width="44.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="51" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="52"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -34785,174 +35130,71 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="60">
-        <v>8</v>
+    <row r="3" spans="1:6" ht="81" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="50">
+        <v>12</v>
       </c>
-      <c r="B3" s="48"/>
-      <c r="C3" s="49" t="s">
+      <c r="B3" s="45" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" s="45" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="45" t="s">
+        <v>71</v>
+      </c>
+      <c r="E3" s="46" t="s">
+        <v>87</v>
+      </c>
+      <c r="F3" s="46" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="50">
+        <v>13</v>
+      </c>
+      <c r="B4" s="45" t="s">
+        <v>85</v>
+      </c>
+      <c r="C4" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="49" t="s">
-        <v>60</v>
+      <c r="D4" s="45" t="s">
+        <v>71</v>
       </c>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-    </row>
-    <row r="4" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="60">
-        <v>9</v>
+      <c r="E4" s="46" t="s">
+        <v>89</v>
       </c>
-      <c r="B4" s="48"/>
-      <c r="C4" s="49" t="s">
-        <v>5</v>
+      <c r="F4" s="46" t="s">
+        <v>90</v>
       </c>
-      <c r="D4" s="49" t="s">
-        <v>60</v>
-      </c>
-      <c r="E4" s="51"/>
-      <c r="F4" s="51"/>
-    </row>
-    <row r="5" spans="1:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="60">
-        <v>10</v>
-      </c>
-      <c r="B5" s="48"/>
-      <c r="C5" s="49" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="49" t="s">
-        <v>60</v>
-      </c>
-      <c r="E5" s="51"/>
-      <c r="F5" s="51"/>
-    </row>
-    <row r="6" spans="1:6" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="60">
-        <v>11</v>
-      </c>
-      <c r="B6" s="48"/>
-      <c r="C6" s="49" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="49" t="s">
-        <v>60</v>
-      </c>
-      <c r="E6" s="51"/>
-      <c r="F6" s="50"/>
-    </row>
-    <row r="8" spans="1:6" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="21"/>
-      <c r="B12" s="21"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-    </row>
-    <row r="13" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="21"/>
-      <c r="B13" s="21"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="21"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:B1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="35.7109375" customWidth="1"/>
-    <col min="5" max="5" width="35.5703125" customWidth="1"/>
-    <col min="6" max="6" width="35.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="54" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-    </row>
-    <row r="2" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="60">
-        <v>12</v>
-      </c>
-      <c r="B3" s="48"/>
-      <c r="C3" s="49" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="49" t="s">
-        <v>60</v>
-      </c>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-    </row>
-    <row r="4" spans="1:6" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="60">
-        <v>13</v>
-      </c>
-      <c r="B4" s="48"/>
-      <c r="C4" s="49" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="49" t="s">
-        <v>60</v>
-      </c>
-      <c r="E4" s="51"/>
-      <c r="F4" s="51"/>
-    </row>
-    <row r="5" spans="1:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="60">
+    </row>
+    <row r="5" spans="1:6" ht="69" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="50">
         <v>14</v>
       </c>
-      <c r="B5" s="48"/>
-      <c r="C5" s="49" t="s">
+      <c r="B5" s="45" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="49" t="s">
-        <v>60</v>
+      <c r="D5" s="45" t="s">
+        <v>40</v>
       </c>
-      <c r="E5" s="51"/>
-      <c r="F5" s="51"/>
+      <c r="E5" s="46" t="s">
+        <v>91</v>
+      </c>
+      <c r="F5" s="46" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B7" s="10"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B9" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>